<commit_message>
Built okay (but not great) python json generator. It leaves trailing in commas in JSON arrays, which is sloppy
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
-    <t>Verb</t>
-  </si>
-  <si>
     <t>Root</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>to close</t>
+  </si>
+  <si>
+    <t>#Verb</t>
   </si>
 </sst>
 </file>
@@ -550,9 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -564,261 +562,261 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
         <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>